<commit_message>
test-20: 2Y error and signif.
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-20.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-20.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="27">
   <si>
     <t>train (MAE)</t>
   </si>
@@ -95,6 +95,12 @@
   </si>
   <si>
     <t>Random Forest-100 (superdataset-24-f 2Y.csv)</t>
+  </si>
+  <si>
+    <t>train (MSE)</t>
+  </si>
+  <si>
+    <t>test (MSE)</t>
   </si>
 </sst>
 </file>
@@ -473,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:J57"/>
+  <dimension ref="C3:T57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,9 +491,12 @@
     <col min="5" max="5" width="12.5703125" customWidth="1"/>
     <col min="9" max="9" width="12.85546875" customWidth="1"/>
     <col min="10" max="10" width="12.7109375" customWidth="1"/>
+    <col min="14" max="14" width="14.28515625" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" customWidth="1"/>
+    <col min="19" max="20" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
@@ -496,8 +505,16 @@
         <v>24</v>
       </c>
       <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="M3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O3" s="1"/>
+      <c r="R3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T3" s="1"/>
+    </row>
+    <row r="4" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
         <v>0</v>
@@ -512,8 +529,22 @@
       <c r="J4" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="M4" s="2"/>
+      <c r="N4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C5" s="2">
         <v>1</v>
       </c>
@@ -526,10 +557,24 @@
       <c r="H5" s="2">
         <v>1</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I5" s="3">
+        <v>35.835579545454529</v>
+      </c>
+      <c r="J5" s="3">
+        <v>93.776145454545443</v>
+      </c>
+      <c r="M5" s="2">
+        <v>1</v>
+      </c>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="R5" s="2">
+        <v>1</v>
+      </c>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+    </row>
+    <row r="6" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C6" s="2">
         <f>C5+1</f>
         <v>2</v>
@@ -544,10 +589,26 @@
         <f>H5+1</f>
         <v>2</v>
       </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-    </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I6" s="3">
+        <v>35.626088636363633</v>
+      </c>
+      <c r="J6" s="3">
+        <v>96.228118181818175</v>
+      </c>
+      <c r="M6" s="2">
+        <f>M5+1</f>
+        <v>2</v>
+      </c>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="R6" s="2">
+        <f>R5+1</f>
+        <v>2</v>
+      </c>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+    </row>
+    <row r="7" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C7" s="2">
         <f t="shared" ref="C7:C54" si="0">C6+1</f>
         <v>3</v>
@@ -562,10 +623,26 @@
         <f t="shared" ref="H7:H54" si="1">H6+1</f>
         <v>3</v>
       </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-    </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I7" s="3">
+        <v>35.101438636363618</v>
+      </c>
+      <c r="J7" s="3">
+        <v>97.568399999999997</v>
+      </c>
+      <c r="M7" s="2">
+        <f t="shared" ref="M7:M54" si="2">M6+1</f>
+        <v>3</v>
+      </c>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="R7" s="2">
+        <f t="shared" ref="R7:R54" si="3">R6+1</f>
+        <v>3</v>
+      </c>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+    </row>
+    <row r="8" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C8" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -580,10 +657,26 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-    </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I8" s="3">
+        <v>35.169211363636357</v>
+      </c>
+      <c r="J8" s="3">
+        <v>95.718109090909095</v>
+      </c>
+      <c r="M8" s="2">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="R8" s="2">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+    </row>
+    <row r="9" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -598,10 +691,26 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-    </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I9" s="3">
+        <v>35.168111363636349</v>
+      </c>
+      <c r="J9" s="3">
+        <v>96.456472727272711</v>
+      </c>
+      <c r="M9" s="2">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="R9" s="2">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+    </row>
+    <row r="10" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C10" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -616,10 +725,26 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I10" s="3">
+        <v>35.982068181818171</v>
+      </c>
+      <c r="J10" s="3">
+        <v>92.065490909090897</v>
+      </c>
+      <c r="M10" s="2">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="R10" s="2">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+    </row>
+    <row r="11" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C11" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -634,10 +759,26 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-    </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I11" s="3">
+        <v>35.977472727272712</v>
+      </c>
+      <c r="J11" s="3">
+        <v>93.488299999999981</v>
+      </c>
+      <c r="M11" s="2">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="R11" s="2">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+    </row>
+    <row r="12" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C12" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -652,10 +793,26 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-    </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I12" s="3">
+        <v>35.246588636363633</v>
+      </c>
+      <c r="J12" s="3">
+        <v>100.7944181818182</v>
+      </c>
+      <c r="M12" s="2">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="R12" s="2">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+    </row>
+    <row r="13" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C13" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -670,10 +827,26 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-    </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I13" s="3">
+        <v>35.371634090909083</v>
+      </c>
+      <c r="J13" s="3">
+        <v>97.756636363636346</v>
+      </c>
+      <c r="M13" s="2">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="R13" s="2">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+    </row>
+    <row r="14" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C14" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -688,10 +861,26 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-    </row>
-    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I14" s="3">
+        <v>35.699120454545437</v>
+      </c>
+      <c r="J14" s="3">
+        <v>94.040472727272714</v>
+      </c>
+      <c r="M14" s="2">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="R14" s="2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+    </row>
+    <row r="15" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C15" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -706,10 +895,26 @@
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-    </row>
-    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I15" s="3">
+        <v>35.813027272727268</v>
+      </c>
+      <c r="J15" s="3">
+        <v>93.231018181818172</v>
+      </c>
+      <c r="M15" s="2">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="R15" s="2">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
+    </row>
+    <row r="16" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C16" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -724,10 +929,26 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-    </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I16" s="3">
+        <v>36.270106818181809</v>
+      </c>
+      <c r="J16" s="3">
+        <v>90.795427272727281</v>
+      </c>
+      <c r="M16" s="2">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="R16" s="2">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="S16" s="3"/>
+      <c r="T16" s="3"/>
+    </row>
+    <row r="17" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C17" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -742,10 +963,26 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-    </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I17" s="3">
+        <v>36.000879545454538</v>
+      </c>
+      <c r="J17" s="3">
+        <v>93.35099090909091</v>
+      </c>
+      <c r="M17" s="2">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="R17" s="2">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="S17" s="3"/>
+      <c r="T17" s="3"/>
+    </row>
+    <row r="18" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C18" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -760,10 +997,26 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-    </row>
-    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I18" s="3">
+        <v>35.908431818181803</v>
+      </c>
+      <c r="J18" s="3">
+        <v>92.774845454545442</v>
+      </c>
+      <c r="M18" s="2">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="R18" s="2">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="S18" s="3"/>
+      <c r="T18" s="3"/>
+    </row>
+    <row r="19" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C19" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -778,10 +1031,26 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-    </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I19" s="3">
+        <v>35.901611363636349</v>
+      </c>
+      <c r="J19" s="3">
+        <v>98.394345454545459</v>
+      </c>
+      <c r="M19" s="2">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="R19" s="2">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="S19" s="3"/>
+      <c r="T19" s="3"/>
+    </row>
+    <row r="20" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C20" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -796,10 +1065,26 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-    </row>
-    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I20" s="3">
+        <v>35.059749999999987</v>
+      </c>
+      <c r="J20" s="3">
+        <v>97.497354545454542</v>
+      </c>
+      <c r="M20" s="2">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="R20" s="2">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="S20" s="3"/>
+      <c r="T20" s="3"/>
+    </row>
+    <row r="21" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C21" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -814,10 +1099,26 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-    </row>
-    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I21" s="3">
+        <v>35.156100000000002</v>
+      </c>
+      <c r="J21" s="3">
+        <v>99.378790909090895</v>
+      </c>
+      <c r="M21" s="2">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="R21" s="2">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
+    </row>
+    <row r="22" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C22" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -832,10 +1133,26 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-    </row>
-    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I22" s="3">
+        <v>35.747754545454526</v>
+      </c>
+      <c r="J22" s="3">
+        <v>93.498299999999986</v>
+      </c>
+      <c r="M22" s="2">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="R22" s="2">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="S22" s="3"/>
+      <c r="T22" s="3"/>
+    </row>
+    <row r="23" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C23" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -850,10 +1167,26 @@
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-    </row>
-    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I23" s="3">
+        <v>35.874429545454547</v>
+      </c>
+      <c r="J23" s="3">
+        <v>96.582918181818172</v>
+      </c>
+      <c r="M23" s="2">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="R23" s="2">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="S23" s="3"/>
+      <c r="T23" s="3"/>
+    </row>
+    <row r="24" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C24" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -868,10 +1201,26 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-    </row>
-    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I24" s="3">
+        <v>35.780704545454533</v>
+      </c>
+      <c r="J24" s="3">
+        <v>95.602736363636339</v>
+      </c>
+      <c r="M24" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="R24" s="2">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="S24" s="3"/>
+      <c r="T24" s="3"/>
+    </row>
+    <row r="25" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C25" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -886,10 +1235,26 @@
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-    </row>
-    <row r="26" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I25" s="3">
+        <v>35.142252272727269</v>
+      </c>
+      <c r="J25" s="3">
+        <v>101.8183090909091</v>
+      </c>
+      <c r="M25" s="2">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="R25" s="2">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="S25" s="3"/>
+      <c r="T25" s="3"/>
+    </row>
+    <row r="26" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C26" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -904,10 +1269,26 @@
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-    </row>
-    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I26" s="3">
+        <v>35.584597727272723</v>
+      </c>
+      <c r="J26" s="3">
+        <v>94.089045454545442</v>
+      </c>
+      <c r="M26" s="2">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="R26" s="2">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="S26" s="3"/>
+      <c r="T26" s="3"/>
+    </row>
+    <row r="27" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C27" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -922,10 +1303,26 @@
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-    </row>
-    <row r="28" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I27" s="3">
+        <v>35.565631818181807</v>
+      </c>
+      <c r="J27" s="3">
+        <v>99.450818181818178</v>
+      </c>
+      <c r="M27" s="2">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="R27" s="2">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="S27" s="3"/>
+      <c r="T27" s="3"/>
+    </row>
+    <row r="28" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C28" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -940,10 +1337,26 @@
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-    </row>
-    <row r="29" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I28" s="3">
+        <v>35.76767499999999</v>
+      </c>
+      <c r="J28" s="3">
+        <v>98.576036363636348</v>
+      </c>
+      <c r="M28" s="2">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="R28" s="2">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="S28" s="3"/>
+      <c r="T28" s="3"/>
+    </row>
+    <row r="29" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C29" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -958,10 +1371,26 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-    </row>
-    <row r="30" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I29" s="3">
+        <v>35.783534090909072</v>
+      </c>
+      <c r="J29" s="3">
+        <v>93.483199999999997</v>
+      </c>
+      <c r="M29" s="2">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="R29" s="2">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="S29" s="3"/>
+      <c r="T29" s="3"/>
+    </row>
+    <row r="30" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C30" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -976,10 +1405,26 @@
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-    </row>
-    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I30" s="3">
+        <v>35.697065909090902</v>
+      </c>
+      <c r="J30" s="3">
+        <v>96.257499999999993</v>
+      </c>
+      <c r="M30" s="2">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+      <c r="R30" s="2">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="S30" s="3"/>
+      <c r="T30" s="3"/>
+    </row>
+    <row r="31" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C31" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -994,10 +1439,26 @@
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-    </row>
-    <row r="32" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I31" s="3">
+        <v>35.342300000000002</v>
+      </c>
+      <c r="J31" s="3">
+        <v>98.202981818181797</v>
+      </c>
+      <c r="M31" s="2">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+      <c r="R31" s="2">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="S31" s="3"/>
+      <c r="T31" s="3"/>
+    </row>
+    <row r="32" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C32" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1012,10 +1473,26 @@
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
-    </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I32" s="3">
+        <v>35.676777272727257</v>
+      </c>
+      <c r="J32" s="3">
+        <v>99.450327272727264</v>
+      </c>
+      <c r="M32" s="2">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+      <c r="R32" s="2">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="S32" s="3"/>
+      <c r="T32" s="3"/>
+    </row>
+    <row r="33" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C33" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1030,10 +1507,26 @@
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-    </row>
-    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I33" s="3">
+        <v>35.929956818181807</v>
+      </c>
+      <c r="J33" s="3">
+        <v>90.835609090909074</v>
+      </c>
+      <c r="M33" s="2">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+      <c r="R33" s="2">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="S33" s="3"/>
+      <c r="T33" s="3"/>
+    </row>
+    <row r="34" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C34" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1048,10 +1541,26 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
-    </row>
-    <row r="35" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I34" s="3">
+        <v>36.24679318181817</v>
+      </c>
+      <c r="J34" s="3">
+        <v>87.894718181818178</v>
+      </c>
+      <c r="M34" s="2">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+      <c r="R34" s="2">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="S34" s="3"/>
+      <c r="T34" s="3"/>
+    </row>
+    <row r="35" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C35" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -1066,10 +1575,26 @@
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-    </row>
-    <row r="36" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I35" s="3">
+        <v>35.170486363636357</v>
+      </c>
+      <c r="J35" s="3">
+        <v>97.195499999999996</v>
+      </c>
+      <c r="M35" s="2">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3"/>
+      <c r="R35" s="2">
+        <f t="shared" si="3"/>
+        <v>31</v>
+      </c>
+      <c r="S35" s="3"/>
+      <c r="T35" s="3"/>
+    </row>
+    <row r="36" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C36" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -1084,10 +1609,26 @@
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
-    </row>
-    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I36" s="3">
+        <v>36.13165681818181</v>
+      </c>
+      <c r="J36" s="3">
+        <v>99.096972727272714</v>
+      </c>
+      <c r="M36" s="2">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="N36" s="3"/>
+      <c r="O36" s="3"/>
+      <c r="R36" s="2">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="S36" s="3"/>
+      <c r="T36" s="3"/>
+    </row>
+    <row r="37" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C37" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -1102,10 +1643,26 @@
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-    </row>
-    <row r="38" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I37" s="3">
+        <v>35.393715909090901</v>
+      </c>
+      <c r="J37" s="3">
+        <v>96.738972727272724</v>
+      </c>
+      <c r="M37" s="2">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="N37" s="3"/>
+      <c r="O37" s="3"/>
+      <c r="R37" s="2">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+      <c r="S37" s="3"/>
+      <c r="T37" s="3"/>
+    </row>
+    <row r="38" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C38" s="2">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1120,10 +1677,26 @@
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
-    </row>
-    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I38" s="3">
+        <v>35.863140909090902</v>
+      </c>
+      <c r="J38" s="3">
+        <v>96.571427272727263</v>
+      </c>
+      <c r="M38" s="2">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="N38" s="3"/>
+      <c r="O38" s="3"/>
+      <c r="R38" s="2">
+        <f t="shared" si="3"/>
+        <v>34</v>
+      </c>
+      <c r="S38" s="3"/>
+      <c r="T38" s="3"/>
+    </row>
+    <row r="39" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C39" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -1138,10 +1711,26 @@
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
-    </row>
-    <row r="40" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I39" s="3">
+        <v>35.649934090909078</v>
+      </c>
+      <c r="J39" s="3">
+        <v>96.245263636363617</v>
+      </c>
+      <c r="M39" s="2">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
+      <c r="R39" s="2">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="S39" s="3"/>
+      <c r="T39" s="3"/>
+    </row>
+    <row r="40" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C40" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1156,10 +1745,26 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
-    </row>
-    <row r="41" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I40" s="3">
+        <v>35.372643181818169</v>
+      </c>
+      <c r="J40" s="3">
+        <v>97.011963636363632</v>
+      </c>
+      <c r="M40" s="2">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="N40" s="3"/>
+      <c r="O40" s="3"/>
+      <c r="R40" s="2">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="S40" s="3"/>
+      <c r="T40" s="3"/>
+    </row>
+    <row r="41" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C41" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -1174,10 +1779,26 @@
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
-    </row>
-    <row r="42" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I41" s="3">
+        <v>35.879179545454527</v>
+      </c>
+      <c r="J41" s="3">
+        <v>95.521627272727272</v>
+      </c>
+      <c r="M41" s="2">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="N41" s="3"/>
+      <c r="O41" s="3"/>
+      <c r="R41" s="2">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="S41" s="3"/>
+      <c r="T41" s="3"/>
+    </row>
+    <row r="42" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C42" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -1192,10 +1813,26 @@
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-    </row>
-    <row r="43" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I42" s="3">
+        <v>36.1957159090909</v>
+      </c>
+      <c r="J42" s="3">
+        <v>90.773309090909095</v>
+      </c>
+      <c r="M42" s="2">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="N42" s="3"/>
+      <c r="O42" s="3"/>
+      <c r="R42" s="2">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="S42" s="3"/>
+      <c r="T42" s="3"/>
+    </row>
+    <row r="43" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C43" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -1210,10 +1847,26 @@
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
-    </row>
-    <row r="44" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I43" s="3">
+        <v>35.841347727272712</v>
+      </c>
+      <c r="J43" s="3">
+        <v>94.809390909090894</v>
+      </c>
+      <c r="M43" s="2">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="N43" s="3"/>
+      <c r="O43" s="3"/>
+      <c r="R43" s="2">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
+      <c r="S43" s="3"/>
+      <c r="T43" s="3"/>
+    </row>
+    <row r="44" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C44" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -1228,10 +1881,26 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
-    </row>
-    <row r="45" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I44" s="3">
+        <v>36.135284090909067</v>
+      </c>
+      <c r="J44" s="3">
+        <v>91.726818181818174</v>
+      </c>
+      <c r="M44" s="2">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="N44" s="3"/>
+      <c r="O44" s="3"/>
+      <c r="R44" s="2">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="S44" s="3"/>
+      <c r="T44" s="3"/>
+    </row>
+    <row r="45" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C45" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -1246,10 +1915,26 @@
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="I45" s="3"/>
-      <c r="J45" s="3"/>
-    </row>
-    <row r="46" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I45" s="3">
+        <v>35.722163636363632</v>
+      </c>
+      <c r="J45" s="3">
+        <v>97.20441818181817</v>
+      </c>
+      <c r="M45" s="2">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="N45" s="3"/>
+      <c r="O45" s="3"/>
+      <c r="R45" s="2">
+        <f t="shared" si="3"/>
+        <v>41</v>
+      </c>
+      <c r="S45" s="3"/>
+      <c r="T45" s="3"/>
+    </row>
+    <row r="46" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C46" s="2">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -1264,10 +1949,26 @@
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="I46" s="3"/>
-      <c r="J46" s="3"/>
-    </row>
-    <row r="47" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I46" s="3">
+        <v>35.844586363636353</v>
+      </c>
+      <c r="J46" s="3">
+        <v>95.495072727272714</v>
+      </c>
+      <c r="M46" s="2">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="N46" s="3"/>
+      <c r="O46" s="3"/>
+      <c r="R46" s="2">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+      <c r="S46" s="3"/>
+      <c r="T46" s="3"/>
+    </row>
+    <row r="47" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C47" s="2">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -1282,10 +1983,26 @@
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
-    </row>
-    <row r="48" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I47" s="3">
+        <v>36.2395909090909</v>
+      </c>
+      <c r="J47" s="3">
+        <v>87.938218181818158</v>
+      </c>
+      <c r="M47" s="2">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="N47" s="3"/>
+      <c r="O47" s="3"/>
+      <c r="R47" s="2">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="S47" s="3"/>
+      <c r="T47" s="3"/>
+    </row>
+    <row r="48" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C48" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -1300,10 +2017,26 @@
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="I48" s="3"/>
-      <c r="J48" s="3"/>
-    </row>
-    <row r="49" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I48" s="3">
+        <v>35.621484090909078</v>
+      </c>
+      <c r="J48" s="3">
+        <v>93.528318181818179</v>
+      </c>
+      <c r="M48" s="2">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="N48" s="3"/>
+      <c r="O48" s="3"/>
+      <c r="R48" s="2">
+        <f t="shared" si="3"/>
+        <v>44</v>
+      </c>
+      <c r="S48" s="3"/>
+      <c r="T48" s="3"/>
+    </row>
+    <row r="49" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C49" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -1318,10 +2051,26 @@
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="I49" s="3"/>
-      <c r="J49" s="3"/>
-    </row>
-    <row r="50" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I49" s="3">
+        <v>35.891149999999989</v>
+      </c>
+      <c r="J49" s="3">
+        <v>90.676581818181816</v>
+      </c>
+      <c r="M49" s="2">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="N49" s="3"/>
+      <c r="O49" s="3"/>
+      <c r="R49" s="2">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+      <c r="S49" s="3"/>
+      <c r="T49" s="3"/>
+    </row>
+    <row r="50" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C50" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -1336,10 +2085,26 @@
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="I50" s="3"/>
-      <c r="J50" s="3"/>
-    </row>
-    <row r="51" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I50" s="3">
+        <v>35.750249999999987</v>
+      </c>
+      <c r="J50" s="3">
+        <v>94.903609090909072</v>
+      </c>
+      <c r="M50" s="2">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="N50" s="3"/>
+      <c r="O50" s="3"/>
+      <c r="R50" s="2">
+        <f t="shared" si="3"/>
+        <v>46</v>
+      </c>
+      <c r="S50" s="3"/>
+      <c r="T50" s="3"/>
+    </row>
+    <row r="51" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C51" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -1354,10 +2119,26 @@
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
-    </row>
-    <row r="52" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I51" s="3">
+        <v>35.574972727272723</v>
+      </c>
+      <c r="J51" s="3">
+        <v>98.204563636363631</v>
+      </c>
+      <c r="M51" s="2">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="N51" s="3"/>
+      <c r="O51" s="3"/>
+      <c r="R51" s="2">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+      <c r="S51" s="3"/>
+      <c r="T51" s="3"/>
+    </row>
+    <row r="52" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C52" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -1372,10 +2153,26 @@
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="I52" s="3"/>
-      <c r="J52" s="3"/>
-    </row>
-    <row r="53" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I52" s="3">
+        <v>35.633363636363619</v>
+      </c>
+      <c r="J52" s="3">
+        <v>94.692390909090904</v>
+      </c>
+      <c r="M52" s="2">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="N52" s="3"/>
+      <c r="O52" s="3"/>
+      <c r="R52" s="2">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="S52" s="3"/>
+      <c r="T52" s="3"/>
+    </row>
+    <row r="53" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C53" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -1390,10 +2187,26 @@
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="I53" s="3"/>
-      <c r="J53" s="3"/>
-    </row>
-    <row r="54" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I53" s="3">
+        <v>36.310788636363633</v>
+      </c>
+      <c r="J53" s="3">
+        <v>90.538454545454542</v>
+      </c>
+      <c r="M53" s="2">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="N53" s="3"/>
+      <c r="O53" s="3"/>
+      <c r="R53" s="2">
+        <f t="shared" si="3"/>
+        <v>49</v>
+      </c>
+      <c r="S53" s="3"/>
+      <c r="T53" s="3"/>
+    </row>
+    <row r="54" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C54" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -1408,10 +2221,26 @@
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="I54" s="3"/>
-      <c r="J54" s="3"/>
-    </row>
-    <row r="56" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I54" s="3">
+        <v>35.511552272727258</v>
+      </c>
+      <c r="J54" s="3">
+        <v>98.017572727272722</v>
+      </c>
+      <c r="M54" s="2">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="N54" s="3"/>
+      <c r="O54" s="3"/>
+      <c r="R54" s="2">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="S54" s="3"/>
+      <c r="T54" s="3"/>
+    </row>
+    <row r="56" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C56" s="2" t="s">
         <v>2</v>
       </c>
@@ -1426,16 +2255,38 @@
       <c r="H56" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I56" s="3" t="e">
+      <c r="I56" s="3">
         <f>AVERAGE(I5:I54)</f>
+        <v>35.703193999999982</v>
+      </c>
+      <c r="J56" s="3">
+        <f>AVERAGE(J5:J54)</f>
+        <v>95.318965636363643</v>
+      </c>
+      <c r="M56" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N56" s="3" t="e">
+        <f>AVERAGE(N5:N54)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J56" s="3" t="e">
-        <f>AVERAGE(J5:J54)</f>
+      <c r="O56" s="3" t="e">
+        <f>AVERAGE(O5:O54)</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="57" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="R56" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S56" s="3" t="e">
+        <f>AVERAGE(S5:S54)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T56" s="3" t="e">
+        <f>AVERAGE(T5:T54)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="57" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C57" s="2" t="s">
         <v>3</v>
       </c>
@@ -1450,12 +2301,34 @@
       <c r="H57" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I57" s="3" t="e">
+      <c r="I57" s="3">
         <f>_xlfn.STDEV.S(I5:I54)</f>
+        <v>0.33437412120926086</v>
+      </c>
+      <c r="J57" s="3">
+        <f>_xlfn.STDEV.S(J5:J54)</f>
+        <v>3.1595966317665791</v>
+      </c>
+      <c r="M57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N57" s="3" t="e">
+        <f>_xlfn.STDEV.S(N5:N54)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J57" s="3" t="e">
-        <f>_xlfn.STDEV.S(J5:J54)</f>
+      <c r="O57" s="3" t="e">
+        <f>_xlfn.STDEV.S(O5:O54)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="S57" s="3" t="e">
+        <f>_xlfn.STDEV.S(S5:S54)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T57" s="3" t="e">
+        <f>_xlfn.STDEV.S(T5:T54)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1466,10 +2339,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:D41"/>
+  <dimension ref="A4:F41"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1477,6 +2350,8 @@
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1499,6 +2374,9 @@
       <c r="C5" s="3">
         <v>7.1388894352929708E-2</v>
       </c>
+      <c r="D5" s="3">
+        <v>7.5297953219226721E-2</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
@@ -1508,6 +2386,9 @@
       <c r="C6" s="3">
         <v>6.4470159101659569E-2</v>
       </c>
+      <c r="D6" s="3">
+        <v>5.9346088214304038E-2</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
@@ -1517,6 +2398,9 @@
       <c r="C7" s="3">
         <v>6.7707876556377056E-2</v>
       </c>
+      <c r="D7" s="3">
+        <v>7.2630088469440773E-2</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
@@ -1526,6 +2410,9 @@
       <c r="C8" s="3">
         <v>4.6371669523161199E-2</v>
       </c>
+      <c r="D8" s="3">
+        <v>4.5103577218663683E-2</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
@@ -1535,6 +2422,9 @@
       <c r="C9" s="3">
         <v>5.300231715760427E-2</v>
       </c>
+      <c r="D9" s="3">
+        <v>5.2064050405848467E-2</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
@@ -1544,6 +2434,9 @@
       <c r="C10" s="3">
         <v>7.6409838115474832E-2</v>
       </c>
+      <c r="D10" s="3">
+        <v>8.0680765509400773E-2</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
@@ -1553,6 +2446,9 @@
       <c r="C11" s="3">
         <v>5.6139722040872107E-2</v>
       </c>
+      <c r="D11" s="3">
+        <v>5.987358322891894E-2</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
@@ -1562,6 +2458,9 @@
       <c r="C12" s="3">
         <v>5.6431511425019683E-2</v>
       </c>
+      <c r="D12" s="3">
+        <v>4.7239375280772683E-2</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
@@ -1571,6 +2470,9 @@
       <c r="C13" s="3">
         <v>4.647879982952656E-2</v>
       </c>
+      <c r="D13" s="3">
+        <v>4.7402095060868857E-2</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
@@ -1580,6 +2482,9 @@
       <c r="C14" s="3">
         <v>6.1051775385052597E-2</v>
       </c>
+      <c r="D14" s="3">
+        <v>6.9740007649667202E-2</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
@@ -1589,6 +2494,9 @@
       <c r="C15" s="3">
         <v>7.1938387955911121E-2</v>
       </c>
+      <c r="D15" s="3">
+        <v>6.8994958644181537E-2</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
@@ -1598,8 +2506,11 @@
       <c r="C16" s="3">
         <v>6.5808806026058056E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="3">
+        <v>6.9197266835097554E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="6" t="s">
         <v>18</v>
@@ -1607,8 +2518,11 @@
       <c r="C17" s="3">
         <v>6.1264981457860183E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="3">
+        <v>5.8909953146660268E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="6" t="s">
         <v>19</v>
@@ -1616,8 +2530,11 @@
       <c r="C18" s="3">
         <v>7.1746720480670378E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="3">
+        <v>5.956278142554991E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="7" t="s">
         <v>20</v>
@@ -1625,8 +2542,11 @@
       <c r="C19" s="3">
         <v>8.3519911319266879E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="3">
+        <v>8.3331582773955054E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="6" t="s">
         <v>21</v>
@@ -1634,146 +2554,251 @@
       <c r="C20" s="3">
         <v>4.6268629272555817E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="3">
+        <v>5.0625872917443512E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B26" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C26" s="3">
         <v>8.3519911319266879E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E26" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="3">
+        <v>8.3331582773955054E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C27" s="3">
         <v>7.6409838115474832E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E27" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="3">
+        <v>8.0680765509400773E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C28" s="3">
         <v>7.1938387955911121E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E28" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28" s="3">
+        <v>7.5297953219226721E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C29" s="3">
         <v>7.1746720480670378E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E29" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29" s="3">
+        <v>7.2630088469440773E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C30" s="3">
         <v>7.1388894352929708E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E30" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" s="3">
+        <v>6.9740007649667202E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B31" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C31" s="3">
         <v>6.7707876556377056E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E31" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31" s="3">
+        <v>6.9197266835097554E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B32" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C32" s="3">
         <v>6.5808806026058056E-2</v>
       </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E32" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32" s="3">
+        <v>6.8994958644181537E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C33" s="3">
         <v>6.4470159101659569E-2</v>
       </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E33" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" s="3">
+        <v>5.987358322891894E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C34" s="3">
         <v>6.1264981457860183E-2</v>
       </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E34" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F34" s="3">
+        <v>5.956278142554991E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C35" s="3">
         <v>6.1051775385052597E-2</v>
       </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E35" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35" s="3">
+        <v>5.9346088214304038E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C36" s="3">
         <v>5.6431511425019683E-2</v>
       </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E36" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F36" s="3">
+        <v>5.8909953146660268E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C37" s="3">
         <v>5.6139722040872107E-2</v>
       </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E37" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" s="3">
+        <v>5.2064050405848467E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C38" s="3">
         <v>5.300231715760427E-2</v>
       </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E38" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F38" s="3">
+        <v>5.0625872917443512E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C39" s="3">
         <v>4.647879982952656E-2</v>
       </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E39" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F39" s="3">
+        <v>4.7402095060868857E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C40" s="3">
         <v>4.6371669523161199E-2</v>
       </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E40" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" s="3">
+        <v>4.7239375280772683E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C41" s="3">
         <v>4.6268629272555817E-2</v>
       </c>
+      <c r="E41" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="3">
+        <v>4.5103577218663683E-2</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="B26:C41">
-    <sortCondition descending="1" ref="C26:C41"/>
+  <sortState ref="E26:F41">
+    <sortCondition descending="1" ref="F26:F41"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
test-20: 3Y size for all metrics
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-20.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-20.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="mae" sheetId="1" r:id="rId1"/>
@@ -4462,7 +4462,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:O58"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="C4" sqref="C4:O58"/>
     </sheetView>
   </sheetViews>
@@ -6189,8 +6189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:O58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="R55" sqref="R55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6244,13 +6244,21 @@
       <c r="C6" s="2">
         <v>1</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="D6" s="3">
+        <v>3216.9870924425632</v>
+      </c>
+      <c r="E6" s="3">
+        <v>25351.210120072548</v>
+      </c>
       <c r="H6" s="2">
         <v>1</v>
       </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
+      <c r="I6" s="3">
+        <v>3045.670391142683</v>
+      </c>
+      <c r="J6" s="3">
+        <v>27046.08139201935</v>
+      </c>
       <c r="M6" s="2">
         <v>1</v>
       </c>
@@ -6266,14 +6274,22 @@
         <f>C6+1</f>
         <v>2</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="D7" s="3">
+        <v>3154.973506166868</v>
+      </c>
+      <c r="E7" s="3">
+        <v>26121.8972496977</v>
+      </c>
       <c r="H7" s="2">
         <f>H6+1</f>
         <v>2</v>
       </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
+      <c r="I7" s="3">
+        <v>3080.5811506045939</v>
+      </c>
+      <c r="J7" s="3">
+        <v>22439.472626964929</v>
+      </c>
       <c r="M7" s="2">
         <f>M6+1</f>
         <v>2</v>
@@ -6290,14 +6306,22 @@
         <f t="shared" ref="C8:C55" si="0">C7+1</f>
         <v>3</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="D8" s="3">
+        <v>3100.3716781741232</v>
+      </c>
+      <c r="E8" s="3">
+        <v>28697.06710278113</v>
+      </c>
       <c r="H8" s="2">
         <f t="shared" ref="H8:H55" si="1">H7+1</f>
         <v>3</v>
       </c>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
+      <c r="I8" s="3">
+        <v>2901.2450577085851</v>
+      </c>
+      <c r="J8" s="3">
+        <v>23917.951183192261</v>
+      </c>
       <c r="M8" s="2">
         <f t="shared" ref="M8:M55" si="2">M7+1</f>
         <v>3</v>
@@ -6314,14 +6338,22 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="D9" s="3">
+        <v>3240.852323458284</v>
+      </c>
+      <c r="E9" s="3">
+        <v>25242.038786577989</v>
+      </c>
       <c r="H9" s="2">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
+      <c r="I9" s="3">
+        <v>3074.1009652660209</v>
+      </c>
+      <c r="J9" s="3">
+        <v>22844.802552962508</v>
+      </c>
       <c r="M9" s="2">
         <f t="shared" si="2"/>
         <v>4</v>
@@ -6338,14 +6370,22 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="D10" s="3">
+        <v>3307.9025003627571</v>
+      </c>
+      <c r="E10" s="3">
+        <v>21073.26174183796</v>
+      </c>
       <c r="H10" s="2">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
+      <c r="I10" s="3">
+        <v>3273.487678415961</v>
+      </c>
+      <c r="J10" s="3">
+        <v>20245.27559866989</v>
+      </c>
       <c r="M10" s="2">
         <f t="shared" si="2"/>
         <v>5</v>
@@ -6362,14 +6402,22 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="D11" s="3">
+        <v>3291.8693716142679</v>
+      </c>
+      <c r="E11" s="3">
+        <v>24302.541663603381</v>
+      </c>
       <c r="H11" s="2">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
+      <c r="I11" s="3">
+        <v>3108.0674021765408</v>
+      </c>
+      <c r="J11" s="3">
+        <v>23408.078405199511</v>
+      </c>
       <c r="M11" s="2">
         <f t="shared" si="2"/>
         <v>6</v>
@@ -6386,14 +6434,22 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+      <c r="D12" s="3">
+        <v>3130.1654001511488</v>
+      </c>
+      <c r="E12" s="3">
+        <v>25536.385920072549</v>
+      </c>
       <c r="H12" s="2">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
+      <c r="I12" s="3">
+        <v>3296.526512817411</v>
+      </c>
+      <c r="J12" s="3">
+        <v>17706.922864691649</v>
+      </c>
       <c r="M12" s="2">
         <f t="shared" si="2"/>
         <v>7</v>
@@ -6410,14 +6466,22 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+      <c r="D13" s="3">
+        <v>3334.504792442563</v>
+      </c>
+      <c r="E13" s="3">
+        <v>24087.751516686811</v>
+      </c>
       <c r="H13" s="2">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
+      <c r="I13" s="3">
+        <v>3229.7577689540499</v>
+      </c>
+      <c r="J13" s="3">
+        <v>19439.272640870611</v>
+      </c>
       <c r="M13" s="2">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -6434,14 +6498,22 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="D14" s="3">
+        <v>3355.074118863361</v>
+      </c>
+      <c r="E14" s="3">
+        <v>21710.85839274486</v>
+      </c>
       <c r="H14" s="2">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
+      <c r="I14" s="3">
+        <v>3077.4802026602169</v>
+      </c>
+      <c r="J14" s="3">
+        <v>24794.033934703752</v>
+      </c>
       <c r="M14" s="2">
         <f t="shared" si="2"/>
         <v>9</v>
@@ -6458,14 +6530,22 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+      <c r="D15" s="3">
+        <v>3221.8093696493352</v>
+      </c>
+      <c r="E15" s="3">
+        <v>24777.486592019341</v>
+      </c>
       <c r="H15" s="2">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
+      <c r="I15" s="3">
+        <v>3102.4045054111239</v>
+      </c>
+      <c r="J15" s="3">
+        <v>22629.07936203144</v>
+      </c>
       <c r="M15" s="2">
         <f t="shared" si="2"/>
         <v>10</v>
@@ -6482,14 +6562,22 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
+      <c r="D16" s="3">
+        <v>3396.0688364570742</v>
+      </c>
+      <c r="E16" s="3">
+        <v>19338.57599455864</v>
+      </c>
       <c r="H16" s="2">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
+      <c r="I16" s="3">
+        <v>3022.8268705562268</v>
+      </c>
+      <c r="J16" s="3">
+        <v>21568.508714873031</v>
+      </c>
       <c r="M16" s="2">
         <f t="shared" si="2"/>
         <v>11</v>
@@ -6506,14 +6594,22 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
+      <c r="D17" s="3">
+        <v>3154.0567938331319</v>
+      </c>
+      <c r="E17" s="3">
+        <v>24617.994903264811</v>
+      </c>
       <c r="H17" s="2">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
+      <c r="I17" s="3">
+        <v>3041.4236683494551</v>
+      </c>
+      <c r="J17" s="3">
+        <v>23575.398734461909</v>
+      </c>
       <c r="M17" s="2">
         <f t="shared" si="2"/>
         <v>12</v>
@@ -6530,14 +6626,22 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
+      <c r="D18" s="3">
+        <v>3245.1017642382112</v>
+      </c>
+      <c r="E18" s="3">
+        <v>24208.241315235791</v>
+      </c>
       <c r="H18" s="2">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
+      <c r="I18" s="3">
+        <v>3130.967229353083</v>
+      </c>
+      <c r="J18" s="3">
+        <v>21726.940821765409</v>
+      </c>
       <c r="M18" s="2">
         <f t="shared" si="2"/>
         <v>13</v>
@@ -6554,14 +6658,22 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
+      <c r="D19" s="3">
+        <v>3397.996879474003</v>
+      </c>
+      <c r="E19" s="3">
+        <v>20916.038330229741</v>
+      </c>
       <c r="H19" s="2">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
+      <c r="I19" s="3">
+        <v>3086.0629383010869</v>
+      </c>
+      <c r="J19" s="3">
+        <v>21996.453624304711</v>
+      </c>
       <c r="M19" s="2">
         <f t="shared" si="2"/>
         <v>14</v>
@@ -6578,14 +6690,22 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
+      <c r="D20" s="3">
+        <v>3400.3085809552608</v>
+      </c>
+      <c r="E20" s="3">
+        <v>22067.07292660217</v>
+      </c>
       <c r="H20" s="2">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
+      <c r="I20" s="3">
+        <v>3094.6658655683191</v>
+      </c>
+      <c r="J20" s="3">
+        <v>23168.47734171704</v>
+      </c>
       <c r="M20" s="2">
         <f t="shared" si="2"/>
         <v>15</v>
@@ -6602,14 +6722,22 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
+      <c r="D21" s="3">
+        <v>3179.3582010580408</v>
+      </c>
+      <c r="E21" s="3">
+        <v>27018.915974365169</v>
+      </c>
       <c r="H21" s="2">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
+      <c r="I21" s="3">
+        <v>3134.8409441354288</v>
+      </c>
+      <c r="J21" s="3">
+        <v>20793.223449334939</v>
+      </c>
       <c r="M21" s="2">
         <f t="shared" si="2"/>
         <v>16</v>
@@ -6626,14 +6754,22 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
+      <c r="D22" s="3">
+        <v>3306.9044490931069</v>
+      </c>
+      <c r="E22" s="3">
+        <v>22842.10722273276</v>
+      </c>
       <c r="H22" s="2">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
+      <c r="I22" s="3">
+        <v>3044.2625793530819</v>
+      </c>
+      <c r="J22" s="3">
+        <v>24005.32559854897</v>
+      </c>
       <c r="M22" s="2">
         <f t="shared" si="2"/>
         <v>17</v>
@@ -6650,14 +6786,22 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
+      <c r="D23" s="3">
+        <v>3115.8719370012091</v>
+      </c>
+      <c r="E23" s="3">
+        <v>27090.224272430471</v>
+      </c>
       <c r="H23" s="2">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
+      <c r="I23" s="3">
+        <v>3092.7339331318012</v>
+      </c>
+      <c r="J23" s="3">
+        <v>21873.356974727929</v>
+      </c>
       <c r="M23" s="2">
         <f t="shared" si="2"/>
         <v>18</v>
@@ -6674,14 +6818,22 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
+      <c r="D24" s="3">
+        <v>3271.5938137847638</v>
+      </c>
+      <c r="E24" s="3">
+        <v>22284.024758041109</v>
+      </c>
       <c r="H24" s="2">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
+      <c r="I24" s="3">
+        <v>3116.78410828295</v>
+      </c>
+      <c r="J24" s="3">
+        <v>23300.082884159609</v>
+      </c>
       <c r="M24" s="2">
         <f t="shared" si="2"/>
         <v>19</v>
@@ -6698,14 +6850,22 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
+      <c r="D25" s="3">
+        <v>3483.1729377871829</v>
+      </c>
+      <c r="E25" s="3">
+        <v>21555.31059673518</v>
+      </c>
       <c r="H25" s="2">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
+      <c r="I25" s="3">
+        <v>3252.620860278113</v>
+      </c>
+      <c r="J25" s="3">
+        <v>18971.207692623939</v>
+      </c>
       <c r="M25" s="2">
         <f t="shared" si="2"/>
         <v>20</v>
@@ -6722,14 +6882,22 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
+      <c r="D26" s="3">
+        <v>3187.9207625755739</v>
+      </c>
+      <c r="E26" s="3">
+        <v>25566.761665659</v>
+      </c>
       <c r="H26" s="2">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
+      <c r="I26" s="3">
+        <v>3056.872164691657</v>
+      </c>
+      <c r="J26" s="3">
+        <v>21584.457699516319</v>
+      </c>
       <c r="M26" s="2">
         <f t="shared" si="2"/>
         <v>21</v>
@@ -6746,14 +6914,22 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
+      <c r="D27" s="3">
+        <v>3480.8487447702541</v>
+      </c>
+      <c r="E27" s="3">
+        <v>20618.276820918982</v>
+      </c>
       <c r="H27" s="2">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
+      <c r="I27" s="3">
+        <v>3197.917487575573</v>
+      </c>
+      <c r="J27" s="3">
+        <v>19761.29710120918</v>
+      </c>
       <c r="M27" s="2">
         <f t="shared" si="2"/>
         <v>22</v>
@@ -6770,14 +6946,22 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
+      <c r="D28" s="3">
+        <v>3441.197816021765</v>
+      </c>
+      <c r="E28" s="3">
+        <v>22556.80917593712</v>
+      </c>
       <c r="H28" s="2">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
+      <c r="I28" s="3">
+        <v>3068.2289293833128</v>
+      </c>
+      <c r="J28" s="3">
+        <v>22698.072636759371</v>
+      </c>
       <c r="M28" s="2">
         <f t="shared" si="2"/>
         <v>23</v>
@@ -6794,14 +6978,22 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
+      <c r="D29" s="3">
+        <v>3259.6399957980648</v>
+      </c>
+      <c r="E29" s="3">
+        <v>25429.238391414739</v>
+      </c>
       <c r="H29" s="2">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
+      <c r="I29" s="3">
+        <v>3087.8486777206772</v>
+      </c>
+      <c r="J29" s="3">
+        <v>21509.049047037479</v>
+      </c>
       <c r="M29" s="2">
         <f t="shared" si="2"/>
         <v>24</v>
@@ -6818,14 +7010,22 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
+      <c r="D30" s="3">
+        <v>3372.943576904474</v>
+      </c>
+      <c r="E30" s="3">
+        <v>22076.55189383313</v>
+      </c>
       <c r="H30" s="2">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
+      <c r="I30" s="3">
+        <v>3081.8367878174122</v>
+      </c>
+      <c r="J30" s="3">
+        <v>21031.092299274489</v>
+      </c>
       <c r="M30" s="2">
         <f t="shared" si="2"/>
         <v>25</v>
@@ -6842,14 +7042,22 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
+      <c r="D31" s="3">
+        <v>3304.854324818622</v>
+      </c>
+      <c r="E31" s="3">
+        <v>25691.617358162031</v>
+      </c>
       <c r="H31" s="2">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
+      <c r="I31" s="3">
+        <v>3145.1498453446179</v>
+      </c>
+      <c r="J31" s="3">
+        <v>18799.522951995161</v>
+      </c>
       <c r="M31" s="2">
         <f t="shared" si="2"/>
         <v>26</v>
@@ -6866,14 +7074,22 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
+      <c r="D32" s="3">
+        <v>3154.557795918985</v>
+      </c>
+      <c r="E32" s="3">
+        <v>24577.280992382101</v>
+      </c>
       <c r="H32" s="2">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
+      <c r="I32" s="3">
+        <v>3047.8011408706152</v>
+      </c>
+      <c r="J32" s="3">
+        <v>23166.169537605801</v>
+      </c>
       <c r="M32" s="2">
         <f t="shared" si="2"/>
         <v>27</v>
@@ -6890,14 +7106,22 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
+      <c r="D33" s="3">
+        <v>3367.8476159915349</v>
+      </c>
+      <c r="E33" s="3">
+        <v>24980.123166989109</v>
+      </c>
       <c r="H33" s="2">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
+      <c r="I33" s="3">
+        <v>3135.6538781438931</v>
+      </c>
+      <c r="J33" s="3">
+        <v>20758.261880532042</v>
+      </c>
       <c r="M33" s="2">
         <f t="shared" si="2"/>
         <v>28</v>
@@ -6914,14 +7138,22 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
+      <c r="D34" s="3">
+        <v>3260.4142163240631</v>
+      </c>
+      <c r="E34" s="3">
+        <v>25114.813624667469</v>
+      </c>
       <c r="H34" s="2">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
+      <c r="I34" s="3">
+        <v>3077.1735257255132</v>
+      </c>
+      <c r="J34" s="3">
+        <v>21649.48267230955</v>
+      </c>
       <c r="M34" s="2">
         <f t="shared" si="2"/>
         <v>29</v>
@@ -6938,14 +7170,22 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
+      <c r="D35" s="3">
+        <v>3224.8080128174129</v>
+      </c>
+      <c r="E35" s="3">
+        <v>23644.69216045949</v>
+      </c>
       <c r="H35" s="2">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
+      <c r="I35" s="3">
+        <v>3075.149316263602</v>
+      </c>
+      <c r="J35" s="3">
+        <v>24549.111314631191</v>
+      </c>
       <c r="M35" s="2">
         <f t="shared" si="2"/>
         <v>30</v>
@@ -6962,14 +7202,22 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
+      <c r="D36" s="3">
+        <v>3309.5213876662629</v>
+      </c>
+      <c r="E36" s="3">
+        <v>25062.871717533249</v>
+      </c>
       <c r="H36" s="2">
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
+      <c r="I36" s="3">
+        <v>3194.785590084643</v>
+      </c>
+      <c r="J36" s="3">
+        <v>21330.725482708582</v>
+      </c>
       <c r="M36" s="2">
         <f t="shared" si="2"/>
         <v>31</v>
@@ -6986,14 +7234,22 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
+      <c r="D37" s="3">
+        <v>3332.2874597339778</v>
+      </c>
+      <c r="E37" s="3">
+        <v>23240.710217775089</v>
+      </c>
       <c r="H37" s="2">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
+      <c r="I37" s="3">
+        <v>3124.9209786577981</v>
+      </c>
+      <c r="J37" s="3">
+        <v>19845.542686094312</v>
+      </c>
       <c r="M37" s="2">
         <f t="shared" si="2"/>
         <v>32</v>
@@ -7010,14 +7266,22 @@
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
+      <c r="D38" s="3">
+        <v>3381.7529509673532</v>
+      </c>
+      <c r="E38" s="3">
+        <v>21502.959778234581</v>
+      </c>
       <c r="H38" s="2">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
+      <c r="I38" s="3">
+        <v>3004.0029480350659</v>
+      </c>
+      <c r="J38" s="3">
+        <v>23979.099173397819</v>
+      </c>
       <c r="M38" s="2">
         <f t="shared" si="2"/>
         <v>33</v>
@@ -7034,14 +7298,22 @@
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
+      <c r="D39" s="3">
+        <v>3268.376077388149</v>
+      </c>
+      <c r="E39" s="3">
+        <v>25027.598042321639</v>
+      </c>
       <c r="H39" s="2">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
+      <c r="I39" s="3">
+        <v>3095.2343067714619</v>
+      </c>
+      <c r="J39" s="3">
+        <v>20299.23827146312</v>
+      </c>
       <c r="M39" s="2">
         <f t="shared" si="2"/>
         <v>34</v>
@@ -7058,14 +7330,22 @@
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
+      <c r="D40" s="3">
+        <v>3311.4699999395411</v>
+      </c>
+      <c r="E40" s="3">
+        <v>23277.425789117289</v>
+      </c>
       <c r="H40" s="2">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
+      <c r="I40" s="3">
+        <v>3168.5234801390561</v>
+      </c>
+      <c r="J40" s="3">
+        <v>20753.645466263599</v>
+      </c>
       <c r="M40" s="2">
         <f t="shared" si="2"/>
         <v>35</v>
@@ -7082,14 +7362,22 @@
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
+      <c r="D41" s="3">
+        <v>3369.1776064691649</v>
+      </c>
+      <c r="E41" s="3">
+        <v>21483.52724244256</v>
+      </c>
       <c r="H41" s="2">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
+      <c r="I41" s="3">
+        <v>3069.061685792019</v>
+      </c>
+      <c r="J41" s="3">
+        <v>24413.13493651753</v>
+      </c>
       <c r="M41" s="2">
         <f t="shared" si="2"/>
         <v>36</v>
@@ -7106,14 +7394,22 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
+      <c r="D42" s="3">
+        <v>3351.5865921704958</v>
+      </c>
+      <c r="E42" s="3">
+        <v>21950.386020435311</v>
+      </c>
       <c r="H42" s="2">
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
+      <c r="I42" s="3">
+        <v>3054.0664550785968</v>
+      </c>
+      <c r="J42" s="3">
+        <v>21997.308454292619</v>
+      </c>
       <c r="M42" s="2">
         <f t="shared" si="2"/>
         <v>37</v>
@@ -7130,14 +7426,22 @@
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
+      <c r="D43" s="3">
+        <v>3418.411057889964</v>
+      </c>
+      <c r="E43" s="3">
+        <v>19416.532257436509</v>
+      </c>
       <c r="H43" s="2">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
+      <c r="I43" s="3">
+        <v>3111.4974358524778</v>
+      </c>
+      <c r="J43" s="3">
+        <v>22067.477231801691</v>
+      </c>
       <c r="M43" s="2">
         <f t="shared" si="2"/>
         <v>38</v>
@@ -7154,14 +7458,22 @@
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
+      <c r="D44" s="3">
+        <v>3358.2446576481261</v>
+      </c>
+      <c r="E44" s="3">
+        <v>22929.82514498186</v>
+      </c>
       <c r="H44" s="2">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
+      <c r="I44" s="3">
+        <v>3164.7610568923819</v>
+      </c>
+      <c r="J44" s="3">
+        <v>21556.806998911728</v>
+      </c>
       <c r="M44" s="2">
         <f t="shared" si="2"/>
         <v>39</v>
@@ -7178,14 +7490,22 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
+      <c r="D45" s="3">
+        <v>3415.787828506649</v>
+      </c>
+      <c r="E45" s="3">
+        <v>22472.83811305925</v>
+      </c>
       <c r="H45" s="2">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="I45" s="3"/>
-      <c r="J45" s="3"/>
+      <c r="I45" s="3">
+        <v>3226.5033131197092</v>
+      </c>
+      <c r="J45" s="3">
+        <v>18173.554329987899</v>
+      </c>
       <c r="M45" s="2">
         <f t="shared" si="2"/>
         <v>40</v>
@@ -7202,14 +7522,22 @@
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
+      <c r="D46" s="3">
+        <v>3355.8406158403868</v>
+      </c>
+      <c r="E46" s="3">
+        <v>23758.70939951632</v>
+      </c>
       <c r="H46" s="2">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="I46" s="3"/>
-      <c r="J46" s="3"/>
+      <c r="I46" s="3">
+        <v>3128.3264233373638</v>
+      </c>
+      <c r="J46" s="3">
+        <v>21767.688337968561</v>
+      </c>
       <c r="M46" s="2">
         <f t="shared" si="2"/>
         <v>41</v>
@@ -7226,14 +7554,22 @@
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
+      <c r="D47" s="3">
+        <v>3397.3991872732759</v>
+      </c>
+      <c r="E47" s="3">
+        <v>21938.229162152358</v>
+      </c>
       <c r="H47" s="2">
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
+      <c r="I47" s="3">
+        <v>3014.7862496977018</v>
+      </c>
+      <c r="J47" s="3">
+        <v>23640.734281015721</v>
+      </c>
       <c r="M47" s="2">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -7250,14 +7586,22 @@
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
+      <c r="D48" s="3">
+        <v>3357.0984856711011</v>
+      </c>
+      <c r="E48" s="3">
+        <v>22992.53917037485</v>
+      </c>
       <c r="H48" s="2">
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="I48" s="3"/>
-      <c r="J48" s="3"/>
+      <c r="I48" s="3">
+        <v>3106.2381782043522</v>
+      </c>
+      <c r="J48" s="3">
+        <v>20609.787174002409</v>
+      </c>
       <c r="M48" s="2">
         <f t="shared" si="2"/>
         <v>43</v>
@@ -7274,14 +7618,22 @@
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
+      <c r="D49" s="3">
+        <v>3328.5219995465532</v>
+      </c>
+      <c r="E49" s="3">
+        <v>26237.459122007251</v>
+      </c>
       <c r="H49" s="2">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="I49" s="3"/>
-      <c r="J49" s="3"/>
+      <c r="I49" s="3">
+        <v>3232.6292698609432</v>
+      </c>
+      <c r="J49" s="3">
+        <v>20846.896878476411</v>
+      </c>
       <c r="M49" s="2">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -7298,14 +7650,22 @@
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
+      <c r="D50" s="3">
+        <v>3341.2638752720682</v>
+      </c>
+      <c r="E50" s="3">
+        <v>22715.359543530831</v>
+      </c>
       <c r="H50" s="2">
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="I50" s="3"/>
-      <c r="J50" s="3"/>
+      <c r="I50" s="3">
+        <v>3075.7291628174121</v>
+      </c>
+      <c r="J50" s="3">
+        <v>23374.509329866982</v>
+      </c>
       <c r="M50" s="2">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -7322,14 +7682,22 @@
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
+      <c r="D51" s="3">
+        <v>3311.3510293228542</v>
+      </c>
+      <c r="E51" s="3">
+        <v>22470.66266311971</v>
+      </c>
       <c r="H51" s="2">
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
+      <c r="I51" s="3">
+        <v>3110.3434353385728</v>
+      </c>
+      <c r="J51" s="3">
+        <v>21763.49903083434</v>
+      </c>
       <c r="M51" s="2">
         <f t="shared" si="2"/>
         <v>46</v>
@@ -7346,14 +7714,22 @@
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
+      <c r="D52" s="3">
+        <v>3386.4982378174118</v>
+      </c>
+      <c r="E52" s="3">
+        <v>20027.732994316801</v>
+      </c>
       <c r="H52" s="2">
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="I52" s="3"/>
-      <c r="J52" s="3"/>
+      <c r="I52" s="3">
+        <v>3121.5836908403862</v>
+      </c>
+      <c r="J52" s="3">
+        <v>20026.41332720677</v>
+      </c>
       <c r="M52" s="2">
         <f t="shared" si="2"/>
         <v>47</v>
@@ -7370,14 +7746,22 @@
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
+      <c r="D53" s="3">
+        <v>3347.7943035368799</v>
+      </c>
+      <c r="E53" s="3">
+        <v>22530.89984691656</v>
+      </c>
       <c r="H53" s="2">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="I53" s="3"/>
-      <c r="J53" s="3"/>
+      <c r="I53" s="3">
+        <v>3098.2479312877872</v>
+      </c>
+      <c r="J53" s="3">
+        <v>21452.670103869401</v>
+      </c>
       <c r="M53" s="2">
         <f t="shared" si="2"/>
         <v>48</v>
@@ -7394,14 +7778,22 @@
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
+      <c r="D54" s="3">
+        <v>3172.8161358827078</v>
+      </c>
+      <c r="E54" s="3">
+        <v>24861.175624909309</v>
+      </c>
       <c r="H54" s="2">
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="I54" s="3"/>
-      <c r="J54" s="3"/>
+      <c r="I54" s="3">
+        <v>3192.224364812575</v>
+      </c>
+      <c r="J54" s="3">
+        <v>19293.88813688029</v>
+      </c>
       <c r="M54" s="2">
         <f t="shared" si="2"/>
         <v>49</v>
@@ -7418,14 +7810,22 @@
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
+      <c r="D55" s="3">
+        <v>3148.306387273276</v>
+      </c>
+      <c r="E55" s="3">
+        <v>25888.576547037479</v>
+      </c>
       <c r="H55" s="2">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="I55" s="3"/>
-      <c r="J55" s="3"/>
+      <c r="I55" s="3">
+        <v>3203.9019245163231</v>
+      </c>
+      <c r="J55" s="3">
+        <v>20743.61531438935</v>
+      </c>
       <c r="M55" s="2">
         <f t="shared" si="2"/>
         <v>50</v>
@@ -7441,24 +7841,24 @@
       <c r="C57" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D57" s="3" t="e">
+      <c r="D57" s="3">
         <f>AVERAGE(D6:D55)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E57" s="3" t="e">
+        <v>3300.4696616952847</v>
+      </c>
+      <c r="E57" s="3">
         <f>AVERAGE(E6:E55)</f>
-        <v>#DIV/0!</v>
+        <v>23577.623780558639</v>
       </c>
       <c r="H57" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I57" s="3" t="e">
+      <c r="I57" s="3">
         <f>AVERAGE(I6:I55)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J57" s="3" t="e">
+        <v>3113.5502053428058</v>
+      </c>
+      <c r="J57" s="3">
         <f>AVERAGE(J6:J55)</f>
-        <v>#DIV/0!</v>
+        <v>21777.853969692856</v>
       </c>
       <c r="M57" s="2" t="s">
         <v>2</v>
@@ -7476,24 +7876,24 @@
       <c r="C58" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D58" s="3" t="e">
+      <c r="D58" s="3">
         <f>_xlfn.STDEV.S(D6:D55)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E58" s="3" t="e">
+        <v>97.570373127286459</v>
+      </c>
+      <c r="E58" s="3">
         <f>_xlfn.STDEV.S(E6:E55)</f>
-        <v>#DIV/0!</v>
+        <v>2072.9251925146796</v>
       </c>
       <c r="H58" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I58" s="3" t="e">
+      <c r="I58" s="3">
         <f>_xlfn.STDEV.S(I6:I55)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J58" s="3" t="e">
+        <v>74.529466313913289</v>
+      </c>
+      <c r="J58" s="3">
         <f>_xlfn.STDEV.S(J6:J55)</f>
-        <v>#DIV/0!</v>
+        <v>1852.100870537872</v>
       </c>
       <c r="M58" s="2" t="s">
         <v>3</v>
@@ -9239,8 +9639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:O58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="Q32" sqref="Q32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9295,8 +9695,12 @@
       <c r="H6" s="2">
         <v>1</v>
       </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
+      <c r="I6" s="3">
+        <v>0.90412555723933363</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0.42750268680290798</v>
+      </c>
       <c r="M6" s="2">
         <v>1</v>
       </c>
@@ -9322,8 +9726,12 @@
         <f>H6+1</f>
         <v>2</v>
       </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
+      <c r="I7" s="3">
+        <v>0.90939255972905075</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0.28052477256734548</v>
+      </c>
       <c r="M7" s="2">
         <f>M6+1</f>
         <v>2</v>
@@ -9350,8 +9758,12 @@
         <f t="shared" ref="H8:H55" si="1">H7+1</f>
         <v>3</v>
       </c>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
+      <c r="I8" s="3">
+        <v>0.91055416855652394</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.27854230234701188</v>
+      </c>
       <c r="M8" s="2">
         <f t="shared" ref="M8:M55" si="2">M7+1</f>
         <v>3</v>
@@ -9378,8 +9790,12 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
+      <c r="I9" s="3">
+        <v>0.90881597568581884</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0.3497551292566905</v>
+      </c>
       <c r="M9" s="2">
         <f t="shared" si="2"/>
         <v>4</v>
@@ -9406,8 +9822,12 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
+      <c r="I10" s="3">
+        <v>0.90911387652511921</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0.35376807502779112</v>
+      </c>
       <c r="M10" s="2">
         <f t="shared" si="2"/>
         <v>5</v>
@@ -9434,8 +9854,12 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
+      <c r="I11" s="3">
+        <v>0.90539514770878049</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0.35355065251754408</v>
+      </c>
       <c r="M11" s="2">
         <f t="shared" si="2"/>
         <v>6</v>
@@ -9462,8 +9886,12 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
+      <c r="I12" s="3">
+        <v>0.90901591236516344</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0.3300243664886775</v>
+      </c>
       <c r="M12" s="2">
         <f t="shared" si="2"/>
         <v>7</v>
@@ -9490,8 +9918,12 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
+      <c r="I13" s="3">
+        <v>0.9079087221562393</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0.28058117093124868</v>
+      </c>
       <c r="M13" s="2">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -9518,8 +9950,12 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
+      <c r="I14" s="3">
+        <v>0.90785397301602544</v>
+      </c>
+      <c r="J14" s="3">
+        <v>0.39191919273441711</v>
+      </c>
       <c r="M14" s="2">
         <f t="shared" si="2"/>
         <v>9</v>
@@ -9546,8 +9982,12 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
+      <c r="I15" s="3">
+        <v>0.90737715026868282</v>
+      </c>
+      <c r="J15" s="3">
+        <v>0.33280952346996717</v>
+      </c>
       <c r="M15" s="2">
         <f t="shared" si="2"/>
         <v>10</v>
@@ -9574,8 +10014,12 @@
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
+      <c r="I16" s="3">
+        <v>0.90823028905856296</v>
+      </c>
+      <c r="J16" s="3">
+        <v>0.34196350840261958</v>
+      </c>
       <c r="M16" s="2">
         <f t="shared" si="2"/>
         <v>11</v>
@@ -9602,8 +10046,12 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
+      <c r="I17" s="3">
+        <v>0.90534639015244911</v>
+      </c>
+      <c r="J17" s="3">
+        <v>0.36590502410462061</v>
+      </c>
       <c r="M17" s="2">
         <f t="shared" si="2"/>
         <v>12</v>
@@ -9630,8 +10078,12 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
+      <c r="I18" s="3">
+        <v>0.91009047458693115</v>
+      </c>
+      <c r="J18" s="3">
+        <v>0.25799876996976823</v>
+      </c>
       <c r="M18" s="2">
         <f t="shared" si="2"/>
         <v>13</v>
@@ -9658,8 +10110,12 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
+      <c r="I19" s="3">
+        <v>0.90929492097599995</v>
+      </c>
+      <c r="J19" s="3">
+        <v>0.32661407871416231</v>
+      </c>
       <c r="M19" s="2">
         <f t="shared" si="2"/>
         <v>14</v>
@@ -9686,8 +10142,12 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
+      <c r="I20" s="3">
+        <v>0.90792311678307247</v>
+      </c>
+      <c r="J20" s="3">
+        <v>0.3178600381297112</v>
+      </c>
       <c r="M20" s="2">
         <f t="shared" si="2"/>
         <v>15</v>
@@ -9714,8 +10174,12 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
+      <c r="I21" s="3">
+        <v>0.90619680558169891</v>
+      </c>
+      <c r="J21" s="3">
+        <v>0.32132652363235858</v>
+      </c>
       <c r="M21" s="2">
         <f t="shared" si="2"/>
         <v>16</v>
@@ -9742,8 +10206,12 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
+      <c r="I22" s="3">
+        <v>0.91123213881750642</v>
+      </c>
+      <c r="J22" s="3">
+        <v>0.37199031296290869</v>
+      </c>
       <c r="M22" s="2">
         <f t="shared" si="2"/>
         <v>17</v>
@@ -9770,8 +10238,12 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
+      <c r="I23" s="3">
+        <v>0.91187704910795719</v>
+      </c>
+      <c r="J23" s="3">
+        <v>0.31878276838904862</v>
+      </c>
       <c r="M23" s="2">
         <f t="shared" si="2"/>
         <v>18</v>
@@ -9798,8 +10270,12 @@
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
+      <c r="I24" s="3">
+        <v>0.90925812610268597</v>
+      </c>
+      <c r="J24" s="3">
+        <v>0.29646399126604911</v>
+      </c>
       <c r="M24" s="2">
         <f t="shared" si="2"/>
         <v>19</v>
@@ -9826,8 +10302,12 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
+      <c r="I25" s="3">
+        <v>0.906255970468544</v>
+      </c>
+      <c r="J25" s="3">
+        <v>0.29727363757154218</v>
+      </c>
       <c r="M25" s="2">
         <f t="shared" si="2"/>
         <v>20</v>
@@ -9854,8 +10334,12 @@
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
+      <c r="I26" s="3">
+        <v>0.9079690878834441</v>
+      </c>
+      <c r="J26" s="3">
+        <v>0.36849869114487532</v>
+      </c>
       <c r="M26" s="2">
         <f t="shared" si="2"/>
         <v>21</v>
@@ -9882,8 +10366,12 @@
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
+      <c r="I27" s="3">
+        <v>0.90866727410770942</v>
+      </c>
+      <c r="J27" s="3">
+        <v>0.27775363877604847</v>
+      </c>
       <c r="M27" s="2">
         <f t="shared" si="2"/>
         <v>22</v>
@@ -9910,8 +10398,12 @@
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
+      <c r="I28" s="3">
+        <v>0.90930927887235624</v>
+      </c>
+      <c r="J28" s="3">
+        <v>0.343630577507264</v>
+      </c>
       <c r="M28" s="2">
         <f t="shared" si="2"/>
         <v>23</v>
@@ -9938,8 +10430,12 @@
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
+      <c r="I29" s="3">
+        <v>0.90547266585714004</v>
+      </c>
+      <c r="J29" s="3">
+        <v>0.34908375181311868</v>
+      </c>
       <c r="M29" s="2">
         <f t="shared" si="2"/>
         <v>24</v>
@@ -9966,8 +10462,12 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
+      <c r="I30" s="3">
+        <v>0.9078507177160523</v>
+      </c>
+      <c r="J30" s="3">
+        <v>0.31702361724545369</v>
+      </c>
       <c r="M30" s="2">
         <f t="shared" si="2"/>
         <v>25</v>
@@ -9994,8 +10494,12 @@
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
+      <c r="I31" s="3">
+        <v>0.91054646095650116</v>
+      </c>
+      <c r="J31" s="3">
+        <v>0.30692973675814178</v>
+      </c>
       <c r="M31" s="2">
         <f t="shared" si="2"/>
         <v>26</v>
@@ -10022,8 +10526,12 @@
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
+      <c r="I32" s="3">
+        <v>0.90904426610177547</v>
+      </c>
+      <c r="J32" s="3">
+        <v>0.3268303380790798</v>
+      </c>
       <c r="M32" s="2">
         <f t="shared" si="2"/>
         <v>27</v>
@@ -10050,8 +10558,12 @@
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
+      <c r="I33" s="3">
+        <v>0.90325833808149991</v>
+      </c>
+      <c r="J33" s="3">
+        <v>0.37223291292966559</v>
+      </c>
       <c r="M33" s="2">
         <f t="shared" si="2"/>
         <v>28</v>
@@ -10078,8 +10590,12 @@
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
+      <c r="I34" s="3">
+        <v>0.90996281054771588</v>
+      </c>
+      <c r="J34" s="3">
+        <v>0.30234599334582413</v>
+      </c>
       <c r="M34" s="2">
         <f t="shared" si="2"/>
         <v>29</v>
@@ -10106,8 +10622,12 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
+      <c r="I35" s="3">
+        <v>0.91197101567459815</v>
+      </c>
+      <c r="J35" s="3">
+        <v>0.29175726336685348</v>
+      </c>
       <c r="M35" s="2">
         <f t="shared" si="2"/>
         <v>30</v>
@@ -10134,8 +10654,12 @@
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
+      <c r="I36" s="3">
+        <v>0.91160163959341389</v>
+      </c>
+      <c r="J36" s="3">
+        <v>0.32560207606498809</v>
+      </c>
       <c r="M36" s="2">
         <f t="shared" si="2"/>
         <v>31</v>
@@ -10162,8 +10686,12 @@
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
+      <c r="I37" s="3">
+        <v>0.91032619961624062</v>
+      </c>
+      <c r="J37" s="3">
+        <v>0.25557868482060792</v>
+      </c>
       <c r="M37" s="2">
         <f t="shared" si="2"/>
         <v>32</v>
@@ -10190,8 +10718,12 @@
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
+      <c r="I38" s="3">
+        <v>0.90649995234227743</v>
+      </c>
+      <c r="J38" s="3">
+        <v>0.38142632022232581</v>
+      </c>
       <c r="M38" s="2">
         <f t="shared" si="2"/>
         <v>33</v>
@@ -10218,8 +10750,12 @@
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
+      <c r="I39" s="3">
+        <v>0.9079017055826375</v>
+      </c>
+      <c r="J39" s="3">
+        <v>0.37956159532344391</v>
+      </c>
       <c r="M39" s="2">
         <f t="shared" si="2"/>
         <v>34</v>
@@ -10246,8 +10782,12 @@
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
+      <c r="I40" s="3">
+        <v>0.90975089215012217</v>
+      </c>
+      <c r="J40" s="3">
+        <v>0.31349251974106551</v>
+      </c>
       <c r="M40" s="2">
         <f t="shared" si="2"/>
         <v>35</v>
@@ -10274,8 +10814,12 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
+      <c r="I41" s="3">
+        <v>0.91005514605582094</v>
+      </c>
+      <c r="J41" s="3">
+        <v>0.34460329470773082</v>
+      </c>
       <c r="M41" s="2">
         <f t="shared" si="2"/>
         <v>36</v>
@@ -10302,8 +10846,12 @@
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
+      <c r="I42" s="3">
+        <v>0.90996706994976218</v>
+      </c>
+      <c r="J42" s="3">
+        <v>0.32837263881826578</v>
+      </c>
       <c r="M42" s="2">
         <f t="shared" si="2"/>
         <v>37</v>
@@ -10330,8 +10878,12 @@
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
+      <c r="I43" s="3">
+        <v>0.90644311154764323</v>
+      </c>
+      <c r="J43" s="3">
+        <v>0.37410656586051089</v>
+      </c>
       <c r="M43" s="2">
         <f t="shared" si="2"/>
         <v>38</v>
@@ -10358,8 +10910,12 @@
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
+      <c r="I44" s="3">
+        <v>0.91034518172196011</v>
+      </c>
+      <c r="J44" s="3">
+        <v>0.33680249949420338</v>
+      </c>
       <c r="M44" s="2">
         <f t="shared" si="2"/>
         <v>39</v>
@@ -10386,8 +10942,12 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="I45" s="3"/>
-      <c r="J45" s="3"/>
+      <c r="I45" s="3">
+        <v>0.90602196001410384</v>
+      </c>
+      <c r="J45" s="3">
+        <v>0.33026211789630988</v>
+      </c>
       <c r="M45" s="2">
         <f t="shared" si="2"/>
         <v>40</v>
@@ -10414,8 +10974,12 @@
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="I46" s="3"/>
-      <c r="J46" s="3"/>
+      <c r="I46" s="3">
+        <v>0.90786779116412131</v>
+      </c>
+      <c r="J46" s="3">
+        <v>0.35652337109062537</v>
+      </c>
       <c r="M46" s="2">
         <f t="shared" si="2"/>
         <v>41</v>
@@ -10442,8 +11006,12 @@
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
+      <c r="I47" s="3">
+        <v>0.90532477036474546</v>
+      </c>
+      <c r="J47" s="3">
+        <v>0.40728237695587011</v>
+      </c>
       <c r="M47" s="2">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -10470,8 +11038,12 @@
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="I48" s="3"/>
-      <c r="J48" s="3"/>
+      <c r="I48" s="3">
+        <v>0.90723085000838521</v>
+      </c>
+      <c r="J48" s="3">
+        <v>0.33864142300859512</v>
+      </c>
       <c r="M48" s="2">
         <f t="shared" si="2"/>
         <v>43</v>
@@ -10498,8 +11070,12 @@
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="I49" s="3"/>
-      <c r="J49" s="3"/>
+      <c r="I49" s="3">
+        <v>0.90451943460731488</v>
+      </c>
+      <c r="J49" s="3">
+        <v>0.35211356528402188</v>
+      </c>
       <c r="M49" s="2">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -10526,8 +11102,12 @@
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="I50" s="3"/>
-      <c r="J50" s="3"/>
+      <c r="I50" s="3">
+        <v>0.90629700275671321</v>
+      </c>
+      <c r="J50" s="3">
+        <v>0.40043933595991321</v>
+      </c>
       <c r="M50" s="2">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -10554,8 +11134,12 @@
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
+      <c r="I51" s="3">
+        <v>0.90859010188473355</v>
+      </c>
+      <c r="J51" s="3">
+        <v>0.31176122208155832</v>
+      </c>
       <c r="M51" s="2">
         <f t="shared" si="2"/>
         <v>46</v>
@@ -10582,8 +11166,12 @@
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="I52" s="3"/>
-      <c r="J52" s="3"/>
+      <c r="I52" s="3">
+        <v>0.90547605896457839</v>
+      </c>
+      <c r="J52" s="3">
+        <v>0.41057111654881329</v>
+      </c>
       <c r="M52" s="2">
         <f t="shared" si="2"/>
         <v>47</v>
@@ -10610,8 +11198,12 @@
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="I53" s="3"/>
-      <c r="J53" s="3"/>
+      <c r="I53" s="3">
+        <v>0.91076257084960499</v>
+      </c>
+      <c r="J53" s="3">
+        <v>0.34449376037067903</v>
+      </c>
       <c r="M53" s="2">
         <f t="shared" si="2"/>
         <v>48</v>
@@ -10638,8 +11230,12 @@
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="I54" s="3"/>
-      <c r="J54" s="3"/>
+      <c r="I54" s="3">
+        <v>0.90777686714993711</v>
+      </c>
+      <c r="J54" s="3">
+        <v>0.30161677552227301</v>
+      </c>
       <c r="M54" s="2">
         <f t="shared" si="2"/>
         <v>49</v>
@@ -10666,8 +11262,12 @@
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="I55" s="3"/>
-      <c r="J55" s="3"/>
+      <c r="I55" s="3">
+        <v>0.90677725150959487</v>
+      </c>
+      <c r="J55" s="3">
+        <v>0.38646012884856662</v>
+      </c>
       <c r="M55" s="2">
         <f t="shared" si="2"/>
         <v>50</v>
@@ -10694,13 +11294,13 @@
       <c r="H57" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I57" s="3" t="e">
+      <c r="I57" s="3">
         <f>AVERAGE(I6:I55)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J57" s="3" t="e">
+        <v>0.90817691597037298</v>
+      </c>
+      <c r="J57" s="3">
         <f>AVERAGE(J6:J55)</f>
-        <v>#DIV/0!</v>
+        <v>0.33661908869746171</v>
       </c>
       <c r="M57" s="2" t="s">
         <v>2</v>
@@ -10729,13 +11329,13 @@
       <c r="H58" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I58" s="3" t="e">
+      <c r="I58" s="3">
         <f>_xlfn.STDEV.S(I6:I55)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J58" s="3" t="e">
+        <v>2.1146529778738312E-3</v>
+      </c>
+      <c r="J58" s="3">
         <f>_xlfn.STDEV.S(J6:J55)</f>
-        <v>#DIV/0!</v>
+        <v>3.9639345196902862E-2</v>
       </c>
       <c r="M58" s="2" t="s">
         <v>3</v>

</xml_diff>